<commit_message>
Update the time zone according to PKR
</commit_message>
<xml_diff>
--- a/scripts/input/threshold.xlsx
+++ b/scripts/input/threshold.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PostEx-Waleed\Desktop\DockerImage\Airflow_Docker\scripts\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADD28542-ED06-4AC3-B989-1EA242AB1A4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{224ADE70-FF66-4820-89E6-2ACDED38E6F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{073B13C2-E5F2-4830-92FA-1DE34A568199}"/>
   </bookViews>
@@ -710,8 +710,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31A5870B-0DB5-4153-B22E-A7AAA7645B90}">
   <dimension ref="A1:B96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
-      <selection activeCell="A98" sqref="A98"/>
+    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="A92" sqref="A92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14"/>

</xml_diff>